<commit_message>
Tracking Stunden dem Terminplan angepasst
</commit_message>
<xml_diff>
--- a/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
+++ b/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E825DFEA-8D7E-46F1-AE16-4D6F61C3A219}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B986D7D-D858-49CD-8DC6-C41C88D75BDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,67 +605,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.23799999999999999</c:v>
+                  <c:v>0.11899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71399999999999997</c:v>
+                  <c:v>0.35699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.19</c:v>
+                  <c:v>0.83299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.3089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.6659999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.1419999999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.6179999999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>2.8559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.0939999999999999</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.0459999999999994</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2839999999999989</c:v>
+                  <c:v>3.4509999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3.5699999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6889999999999992</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8079999999999989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9269999999999987</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0459999999999985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1649999999999983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.283999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>4.5219999999999985</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.9979999999999976</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.2359999999999971</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.4739999999999966</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.7119999999999962</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.9499999999999957</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.4259999999999957</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.9019999999999957</c:v>
+                  <c:v>4.8789999999999987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3779999999999957</c:v>
+                  <c:v>5.2359999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,67 +777,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6319999999999999</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2639999999999998</c:v>
+                  <c:v>1.7000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8959999999999999</c:v>
+                  <c:v>3.0600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5279999999999996</c:v>
+                  <c:v>4.7600000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.16</c:v>
+                  <c:v>6.4600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7919999999999998</c:v>
+                  <c:v>7.48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.016</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,61 +1127,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.0880000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3119999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.88400000000000001</c:v>
+                  <c:v>3.1279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.768</c:v>
+                  <c:v>4.1479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.448</c:v>
+                  <c:v>5.7799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.536</c:v>
+                  <c:v>6.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.032</c:v>
+                  <c:v>8.4319999999999986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5280000000000005</c:v>
+                  <c:v>10.063999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0240000000000009</c:v>
+                  <c:v>11.695999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.5200000000000014</c:v>
+                  <c:v>13.327999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.88</c:v>
+                  <c:v>14.959999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2817,67 +2817,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.23799999999999999</c:v>
+                  <c:v>0.11899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71399999999999997</c:v>
+                  <c:v>0.35699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.19</c:v>
+                  <c:v>0.83299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.3089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.6659999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.1419999999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.6179999999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>2.8559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.0939999999999999</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.0459999999999994</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2839999999999989</c:v>
+                  <c:v>3.4509999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3.5699999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6889999999999992</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8079999999999989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9269999999999987</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0459999999999985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1649999999999983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.283999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>4.5219999999999985</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.9979999999999976</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.2359999999999971</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.4739999999999966</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.7119999999999962</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.9499999999999957</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.4259999999999957</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.9019999999999957</c:v>
+                  <c:v>4.8789999999999987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3779999999999957</c:v>
+                  <c:v>5.2359999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2989,67 +2989,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6319999999999999</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2639999999999998</c:v>
+                  <c:v>1.7000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8959999999999999</c:v>
+                  <c:v>3.0600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5279999999999996</c:v>
+                  <c:v>4.7600000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.16</c:v>
+                  <c:v>6.4600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7919999999999998</c:v>
+                  <c:v>7.48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.016</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3339,61 +3339,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.0880000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3119999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.88400000000000001</c:v>
+                  <c:v>3.1279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.768</c:v>
+                  <c:v>4.1479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.448</c:v>
+                  <c:v>5.7799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.536</c:v>
+                  <c:v>6.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.032</c:v>
+                  <c:v>8.4319999999999986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5280000000000005</c:v>
+                  <c:v>10.063999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0240000000000009</c:v>
+                  <c:v>11.695999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.5200000000000014</c:v>
+                  <c:v>13.327999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.88</c:v>
+                  <c:v>14.959999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5119,67 +5119,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.23799999999999999</c:v>
+                  <c:v>0.11899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71399999999999997</c:v>
+                  <c:v>0.35699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.19</c:v>
+                  <c:v>0.83299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.3089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.6659999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.1419999999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.6179999999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>2.8559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.0939999999999999</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.0459999999999994</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2839999999999989</c:v>
+                  <c:v>3.4509999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3.5699999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6889999999999992</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8079999999999989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9269999999999987</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0459999999999985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1649999999999983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.283999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>4.5219999999999985</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.9979999999999976</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.2359999999999971</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.4739999999999966</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.7119999999999962</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.9499999999999957</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.4259999999999957</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.9019999999999957</c:v>
+                  <c:v>4.8789999999999987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3779999999999957</c:v>
+                  <c:v>5.2359999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5291,67 +5291,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6319999999999999</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2639999999999998</c:v>
+                  <c:v>1.7000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8959999999999999</c:v>
+                  <c:v>3.0600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5279999999999996</c:v>
+                  <c:v>4.7600000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.16</c:v>
+                  <c:v>6.4600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7919999999999998</c:v>
+                  <c:v>7.48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.016</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5641,61 +5641,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.0880000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3119999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.88400000000000001</c:v>
+                  <c:v>3.1279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.768</c:v>
+                  <c:v>4.1479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.448</c:v>
+                  <c:v>5.7799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.536</c:v>
+                  <c:v>6.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.032</c:v>
+                  <c:v>8.4319999999999986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5280000000000005</c:v>
+                  <c:v>10.063999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0240000000000009</c:v>
+                  <c:v>11.695999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.5200000000000014</c:v>
+                  <c:v>13.327999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.88</c:v>
+                  <c:v>14.959999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7529,67 +7529,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.23799999999999999</c:v>
+                  <c:v>0.11899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.71399999999999997</c:v>
+                  <c:v>0.35699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.19</c:v>
+                  <c:v>0.83299999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1.3089999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.6659999999999999</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>2.1419999999999999</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
+                  <c:v>2.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>2.6179999999999999</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="8">
+                  <c:v>2.8559999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>3.0939999999999999</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.57</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4.0459999999999994</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2839999999999989</c:v>
+                  <c:v>3.4509999999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>3.5699999999999994</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.6889999999999992</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.8079999999999989</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9269999999999987</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.0459999999999985</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.1649999999999983</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.283999999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>4.5219999999999985</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.759999999999998</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.9979999999999976</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.2359999999999971</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.4739999999999966</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.7119999999999962</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.9499999999999957</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>6.4259999999999957</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.9019999999999957</c:v>
+                  <c:v>4.8789999999999987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.3779999999999957</c:v>
+                  <c:v>5.2359999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7701,67 +7701,67 @@
                 <c:formatCode>#,##0.0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.6319999999999999</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2639999999999998</c:v>
+                  <c:v>1.7000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8959999999999999</c:v>
+                  <c:v>3.0600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5279999999999996</c:v>
+                  <c:v>4.7600000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.16</c:v>
+                  <c:v>6.4600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.7919999999999998</c:v>
+                  <c:v>7.48</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.016</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.832000000000001</c:v>
+                  <c:v>9.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8051,61 +8051,61 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.0880000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2.3119999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.88400000000000001</c:v>
+                  <c:v>3.1279999999999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.768</c:v>
+                  <c:v>4.1479999999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.448</c:v>
+                  <c:v>5.7799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.536</c:v>
+                  <c:v>6.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.032</c:v>
+                  <c:v>8.4319999999999986</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.5280000000000005</c:v>
+                  <c:v>10.063999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.0240000000000009</c:v>
+                  <c:v>11.695999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.5200000000000014</c:v>
+                  <c:v>13.327999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>10.88</c:v>
+                  <c:v>14.959999999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.88</c:v>
+                  <c:v>15.299999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10311,7 +10311,7 @@
       <pane xSplit="4" ySplit="10" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F103" sqref="F103"/>
+      <selection pane="bottomRight" activeCell="V62" sqref="V62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10506,10 +10506,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17">
         <v>2</v>
-      </c>
-      <c r="F14" s="17">
-        <v>4</v>
       </c>
       <c r="G14" s="17">
         <v>4</v>
@@ -10518,16 +10518,16 @@
         <v>4</v>
       </c>
       <c r="I14" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J14" s="17">
         <v>4</v>
       </c>
       <c r="K14" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L14" s="17">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M14" s="17">
         <v>2</v>
@@ -10536,41 +10536,41 @@
         <v>2</v>
       </c>
       <c r="O14" s="17">
+        <v>3</v>
+      </c>
+      <c r="P14" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>1</v>
+      </c>
+      <c r="R14" s="17">
+        <v>1</v>
+      </c>
+      <c r="S14" s="17">
+        <v>1</v>
+      </c>
+      <c r="T14" s="17">
+        <v>1</v>
+      </c>
+      <c r="U14" s="17">
+        <v>1</v>
+      </c>
+      <c r="V14" s="17">
+        <v>1</v>
+      </c>
+      <c r="W14" s="17">
         <v>2</v>
       </c>
-      <c r="P14" s="17">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="17">
-        <v>2</v>
-      </c>
-      <c r="R14" s="17">
-        <v>2</v>
-      </c>
-      <c r="S14" s="17">
-        <v>2</v>
-      </c>
-      <c r="T14" s="17">
-        <v>2</v>
-      </c>
-      <c r="U14" s="17">
-        <v>2</v>
-      </c>
-      <c r="V14" s="17">
-        <v>2</v>
-      </c>
-      <c r="W14" s="17">
-        <v>4</v>
-      </c>
       <c r="X14" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y14" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA14" s="20">
         <f>SUM(E14:Y14)</f>
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.25">
@@ -10580,87 +10580,87 @@
       <c r="D15" s="6"/>
       <c r="E15" s="18">
         <f>E14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="18">
         <f>E15+F14</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G15" s="18">
         <f>F15+G14</f>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H15" s="18">
         <f t="shared" ref="H15:Y15" si="0">G15+H14</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I15" s="18">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="J15" s="18">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="K15" s="18">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="L15" s="18">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="M15" s="18">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="N15" s="18">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="O15" s="18">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P15" s="18">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="Q15" s="18">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="R15" s="18">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="S15" s="18">
         <f t="shared" si="0"/>
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="T15" s="18">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="U15" s="18">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="V15" s="18">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="W15" s="18">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="X15" s="18">
         <f t="shared" si="0"/>
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="Y15" s="18">
         <f t="shared" si="0"/>
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="AA15" s="5"/>
     </row>
@@ -10673,11 +10673,11 @@
       </c>
       <c r="E16" s="10">
         <f>E14*$D$6/1000</f>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="F16" s="10">
         <f>F14*$D$6/1000</f>
-        <v>0.47599999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" ref="G16:Y16" si="1">G14*$D$6/1000</f>
@@ -10689,7 +10689,7 @@
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="J16" s="10">
         <f t="shared" si="1"/>
@@ -10697,11 +10697,11 @@
       </c>
       <c r="K16" s="10">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="L16" s="10">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="M16" s="10">
         <f t="shared" si="1"/>
@@ -10713,51 +10713,51 @@
       </c>
       <c r="O16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="P16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="Q16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="R16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="S16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="T16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="U16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="V16" s="10">
         <f t="shared" si="1"/>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="W16" s="10">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.23799999999999999</v>
       </c>
       <c r="X16" s="10">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="Y16" s="10">
         <f t="shared" si="1"/>
-        <v>0.47599999999999998</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="AA16" s="10">
         <f>SUM(E16:Y16)</f>
-        <v>7.3779999999999957</v>
+        <v>5.2359999999999989</v>
       </c>
     </row>
     <row r="17" spans="2:27" x14ac:dyDescent="0.25">
@@ -10772,87 +10772,87 @@
       </c>
       <c r="E17" s="10">
         <f>E16</f>
-        <v>0.23799999999999999</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="F17" s="10">
         <f>E17+F16</f>
-        <v>0.71399999999999997</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" ref="G17:Y17" si="2">F17+G16</f>
-        <v>1.19</v>
+        <v>0.83299999999999996</v>
       </c>
       <c r="H17" s="10">
         <f t="shared" si="2"/>
-        <v>1.6659999999999999</v>
+        <v>1.3089999999999999</v>
       </c>
       <c r="I17" s="10">
         <f t="shared" si="2"/>
-        <v>2.1419999999999999</v>
+        <v>1.6659999999999999</v>
       </c>
       <c r="J17" s="10">
         <f t="shared" si="2"/>
-        <v>2.6179999999999999</v>
+        <v>2.1419999999999999</v>
       </c>
       <c r="K17" s="10">
         <f t="shared" si="2"/>
-        <v>3.0939999999999999</v>
+        <v>2.38</v>
       </c>
       <c r="L17" s="10">
         <f t="shared" si="2"/>
-        <v>3.57</v>
+        <v>2.6179999999999999</v>
       </c>
       <c r="M17" s="10">
         <f t="shared" si="2"/>
-        <v>3.8079999999999998</v>
+        <v>2.8559999999999999</v>
       </c>
       <c r="N17" s="10">
         <f t="shared" si="2"/>
-        <v>4.0459999999999994</v>
+        <v>3.0939999999999999</v>
       </c>
       <c r="O17" s="10">
         <f t="shared" si="2"/>
-        <v>4.2839999999999989</v>
+        <v>3.4509999999999996</v>
       </c>
       <c r="P17" s="10">
         <f t="shared" si="2"/>
-        <v>4.5219999999999985</v>
+        <v>3.5699999999999994</v>
       </c>
       <c r="Q17" s="10">
         <f t="shared" si="2"/>
-        <v>4.759999999999998</v>
+        <v>3.6889999999999992</v>
       </c>
       <c r="R17" s="10">
         <f t="shared" si="2"/>
-        <v>4.9979999999999976</v>
+        <v>3.8079999999999989</v>
       </c>
       <c r="S17" s="10">
         <f t="shared" si="2"/>
-        <v>5.2359999999999971</v>
+        <v>3.9269999999999987</v>
       </c>
       <c r="T17" s="10">
         <f t="shared" si="2"/>
-        <v>5.4739999999999966</v>
+        <v>4.0459999999999985</v>
       </c>
       <c r="U17" s="10">
         <f t="shared" si="2"/>
-        <v>5.7119999999999962</v>
+        <v>4.1649999999999983</v>
       </c>
       <c r="V17" s="10">
         <f t="shared" si="2"/>
-        <v>5.9499999999999957</v>
+        <v>4.283999999999998</v>
       </c>
       <c r="W17" s="10">
         <f t="shared" si="2"/>
-        <v>6.4259999999999957</v>
+        <v>4.5219999999999985</v>
       </c>
       <c r="X17" s="10">
         <f t="shared" si="2"/>
-        <v>6.9019999999999957</v>
+        <v>4.8789999999999987</v>
       </c>
       <c r="Y17" s="10">
         <f t="shared" si="2"/>
-        <v>7.3779999999999957</v>
+        <v>5.2359999999999989</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.25">
@@ -11355,28 +11355,28 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="17">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F28" s="17">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G28" s="17">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="H28" s="17">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I28" s="17">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J28" s="17">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K28" s="17">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="L28" s="17">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
@@ -11393,7 +11393,7 @@
       <c r="Y28" s="17"/>
       <c r="AA28" s="20">
         <f>SUM(E28:Y28)</f>
-        <v>174</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
@@ -11403,87 +11403,87 @@
       <c r="D29" s="6"/>
       <c r="E29" s="18">
         <f>E28</f>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F29" s="18">
         <f>E29+F28</f>
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="G29" s="18">
         <f>F29+G28</f>
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="H29" s="18">
         <f t="shared" ref="H29" si="38">G29+H28</f>
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="I29" s="18">
         <f t="shared" ref="I29" si="39">H29+I28</f>
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="J29" s="18">
         <f t="shared" ref="J29" si="40">I29+J28</f>
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="K29" s="18">
         <f t="shared" ref="K29" si="41">J29+K28</f>
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="L29" s="18">
         <f t="shared" ref="L29" si="42">K29+L28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="M29" s="18">
         <f t="shared" ref="M29" si="43">L29+M28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="N29" s="18">
         <f t="shared" ref="N29" si="44">M29+N28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="O29" s="18">
         <f t="shared" ref="O29" si="45">N29+O28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="P29" s="18">
         <f t="shared" ref="P29" si="46">O29+P28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="Q29" s="18">
         <f t="shared" ref="Q29" si="47">P29+Q28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="R29" s="18">
         <f t="shared" ref="R29" si="48">Q29+R28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="S29" s="18">
         <f t="shared" ref="S29" si="49">R29+S28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="T29" s="18">
         <f t="shared" ref="T29" si="50">S29+T28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="U29" s="18">
         <f t="shared" ref="U29" si="51">T29+U28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="V29" s="18">
         <f t="shared" ref="V29" si="52">U29+V28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="W29" s="18">
         <f t="shared" ref="W29" si="53">V29+W28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="X29" s="18">
         <f t="shared" ref="X29" si="54">W29+X28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="Y29" s="18">
         <f t="shared" ref="Y29" si="55">X29+Y28</f>
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="AA29" s="5"/>
     </row>
@@ -11496,35 +11496,35 @@
       </c>
       <c r="E30" s="10">
         <f>E28*$D$7/1000</f>
-        <v>1.6319999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="F30" s="10">
         <f>F28*$D$7/1000</f>
-        <v>1.6319999999999999</v>
+        <v>1.02</v>
       </c>
       <c r="G30" s="10">
         <f t="shared" ref="G30:Y30" si="56">G28*$D$7/1000</f>
-        <v>1.6319999999999999</v>
+        <v>1.36</v>
       </c>
       <c r="H30" s="10">
         <f t="shared" si="56"/>
-        <v>1.6319999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="I30" s="10">
         <f t="shared" si="56"/>
-        <v>1.6319999999999999</v>
+        <v>1.7</v>
       </c>
       <c r="J30" s="10">
         <f t="shared" si="56"/>
-        <v>1.6319999999999999</v>
+        <v>1.02</v>
       </c>
       <c r="K30" s="10">
         <f t="shared" si="56"/>
-        <v>1.224</v>
+        <v>1.02</v>
       </c>
       <c r="L30" s="10">
         <f t="shared" si="56"/>
-        <v>0.81599999999999995</v>
+        <v>0.68</v>
       </c>
       <c r="M30" s="10">
         <f t="shared" si="56"/>
@@ -11580,7 +11580,7 @@
       </c>
       <c r="AA30" s="10">
         <f>SUM(E30:Y30)</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
     </row>
     <row r="31" spans="2:27" x14ac:dyDescent="0.25">
@@ -11595,87 +11595,87 @@
       </c>
       <c r="E31" s="10">
         <f>E30</f>
-        <v>1.6319999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="F31" s="10">
         <f>E31+F30</f>
-        <v>3.2639999999999998</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="G31" s="10">
         <f t="shared" ref="G31" si="57">F31+G30</f>
-        <v>4.8959999999999999</v>
+        <v>3.0600000000000005</v>
       </c>
       <c r="H31" s="10">
         <f t="shared" ref="H31" si="58">G31+H30</f>
-        <v>6.5279999999999996</v>
+        <v>4.7600000000000007</v>
       </c>
       <c r="I31" s="10">
         <f t="shared" ref="I31" si="59">H31+I30</f>
-        <v>8.16</v>
+        <v>6.4600000000000009</v>
       </c>
       <c r="J31" s="10">
         <f t="shared" ref="J31" si="60">I31+J30</f>
-        <v>9.7919999999999998</v>
+        <v>7.48</v>
       </c>
       <c r="K31" s="10">
         <f t="shared" ref="K31" si="61">J31+K30</f>
-        <v>11.016</v>
+        <v>8.5</v>
       </c>
       <c r="L31" s="10">
         <f t="shared" ref="L31" si="62">K31+L30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="M31" s="10">
         <f t="shared" ref="M31" si="63">L31+M30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="N31" s="10">
         <f t="shared" ref="N31" si="64">M31+N30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="O31" s="10">
         <f t="shared" ref="O31" si="65">N31+O30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="P31" s="10">
         <f t="shared" ref="P31" si="66">O31+P30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="Q31" s="10">
         <f t="shared" ref="Q31" si="67">P31+Q30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="R31" s="10">
         <f t="shared" ref="R31" si="68">Q31+R30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="S31" s="10">
         <f t="shared" ref="S31" si="69">R31+S30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="T31" s="10">
         <f t="shared" ref="T31" si="70">S31+T30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="U31" s="10">
         <f t="shared" ref="U31" si="71">T31+U30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="V31" s="10">
         <f t="shared" ref="V31" si="72">U31+V30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="W31" s="10">
         <f t="shared" ref="W31" si="73">V31+W30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="X31" s="10">
         <f t="shared" ref="X31" si="74">W31+X30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
       <c r="Y31" s="10">
         <f t="shared" ref="Y31" si="75">X31+Y30</f>
-        <v>11.832000000000001</v>
+        <v>9.18</v>
       </c>
     </row>
     <row r="33" spans="2:27" x14ac:dyDescent="0.25">
@@ -13190,46 +13190,58 @@
       <c r="D62" s="6"/>
       <c r="E62" s="17"/>
       <c r="F62" s="17"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
-      <c r="J62" s="17"/>
-      <c r="K62" s="17"/>
+      <c r="G62" s="17">
+        <v>5</v>
+      </c>
+      <c r="H62" s="17">
+        <v>5</v>
+      </c>
+      <c r="I62" s="17">
+        <v>6</v>
+      </c>
+      <c r="J62" s="17">
+        <v>6</v>
+      </c>
+      <c r="K62" s="17">
+        <v>12</v>
+      </c>
       <c r="L62" s="17">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M62" s="17">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="N62" s="17">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="O62" s="17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P62" s="17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="Q62" s="17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="R62" s="17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="S62" s="17">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="T62" s="17">
-        <v>20</v>
-      </c>
-      <c r="U62" s="17"/>
+        <v>24</v>
+      </c>
+      <c r="U62" s="17">
+        <v>5</v>
+      </c>
       <c r="V62" s="17"/>
       <c r="W62" s="17"/>
       <c r="X62" s="17"/>
       <c r="Y62" s="17"/>
       <c r="AA62" s="20">
         <f>SUM(E62:Y62)</f>
-        <v>160</v>
+        <v>225</v>
       </c>
     </row>
     <row r="63" spans="2:27" x14ac:dyDescent="0.25">
@@ -13247,79 +13259,79 @@
       </c>
       <c r="G63" s="18">
         <f>F63+G62</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H63" s="18">
         <f t="shared" ref="H63" si="234">G63+H62</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I63" s="18">
         <f t="shared" ref="I63" si="235">H63+I62</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="J63" s="18">
         <f t="shared" ref="J63" si="236">I63+J62</f>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="K63" s="18">
         <f t="shared" ref="K63" si="237">J63+K62</f>
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="L63" s="18">
         <f t="shared" ref="L63" si="238">K63+L62</f>
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="M63" s="18">
         <f t="shared" ref="M63" si="239">L63+M62</f>
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="N63" s="18">
         <f t="shared" ref="N63" si="240">M63+N62</f>
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="O63" s="18">
         <f t="shared" ref="O63" si="241">N63+O62</f>
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="P63" s="18">
         <f t="shared" ref="P63" si="242">O63+P62</f>
-        <v>74</v>
+        <v>124</v>
       </c>
       <c r="Q63" s="18">
         <f t="shared" ref="Q63" si="243">P63+Q62</f>
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="R63" s="18">
         <f t="shared" ref="R63" si="244">Q63+R62</f>
-        <v>118</v>
+        <v>172</v>
       </c>
       <c r="S63" s="18">
         <f t="shared" ref="S63" si="245">R63+S62</f>
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="T63" s="18">
         <f t="shared" ref="T63" si="246">S63+T62</f>
-        <v>160</v>
+        <v>220</v>
       </c>
       <c r="U63" s="18">
         <f t="shared" ref="U63" si="247">T63+U62</f>
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="V63" s="18">
         <f t="shared" ref="V63" si="248">U63+V62</f>
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="W63" s="18">
         <f t="shared" ref="W63" si="249">V63+W62</f>
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="X63" s="18">
         <f t="shared" ref="X63" si="250">W63+X62</f>
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="Y63" s="18">
         <f t="shared" ref="Y63" si="251">X63+Y62</f>
-        <v>160</v>
+        <v>225</v>
       </c>
       <c r="AA63" s="5"/>
     </row>
@@ -13340,63 +13352,63 @@
       </c>
       <c r="G64" s="10">
         <f t="shared" ref="G64:Y64" si="252">G62*$D$7/1000</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="H64" s="10">
         <f t="shared" si="252"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="I64" s="10">
         <f t="shared" si="252"/>
-        <v>0</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="J64" s="10">
         <f t="shared" si="252"/>
-        <v>0</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="K64" s="10">
         <f t="shared" si="252"/>
-        <v>0</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="L64" s="10">
         <f t="shared" si="252"/>
-        <v>0.88400000000000001</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="M64" s="10">
         <f t="shared" si="252"/>
-        <v>0.88400000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="N64" s="10">
         <f t="shared" si="252"/>
-        <v>0.68</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="O64" s="10">
         <f t="shared" si="252"/>
-        <v>1.0880000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="P64" s="10">
         <f t="shared" si="252"/>
-        <v>1.496</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="Q64" s="10">
         <f t="shared" si="252"/>
-        <v>1.496</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="R64" s="10">
         <f t="shared" si="252"/>
-        <v>1.496</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="S64" s="10">
         <f t="shared" si="252"/>
-        <v>1.496</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="T64" s="10">
         <f t="shared" si="252"/>
-        <v>1.36</v>
+        <v>1.6319999999999999</v>
       </c>
       <c r="U64" s="10">
         <f t="shared" si="252"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="V64" s="10">
         <f t="shared" si="252"/>
@@ -13416,7 +13428,7 @@
       </c>
       <c r="AA64" s="10">
         <f>SUM(E64:Y64)</f>
-        <v>10.88</v>
+        <v>15.299999999999997</v>
       </c>
     </row>
     <row r="65" spans="2:27" x14ac:dyDescent="0.25">
@@ -13439,79 +13451,79 @@
       </c>
       <c r="G65" s="10">
         <f t="shared" ref="G65" si="253">F65+G64</f>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="H65" s="10">
         <f t="shared" ref="H65" si="254">G65+H64</f>
-        <v>0</v>
+        <v>0.68</v>
       </c>
       <c r="I65" s="10">
         <f t="shared" ref="I65" si="255">H65+I64</f>
-        <v>0</v>
+        <v>1.0880000000000001</v>
       </c>
       <c r="J65" s="10">
         <f t="shared" ref="J65" si="256">I65+J64</f>
-        <v>0</v>
+        <v>1.496</v>
       </c>
       <c r="K65" s="10">
         <f t="shared" ref="K65" si="257">J65+K64</f>
-        <v>0</v>
+        <v>2.3119999999999998</v>
       </c>
       <c r="L65" s="10">
         <f t="shared" ref="L65" si="258">K65+L64</f>
-        <v>0.88400000000000001</v>
+        <v>3.1279999999999997</v>
       </c>
       <c r="M65" s="10">
         <f t="shared" ref="M65" si="259">L65+M64</f>
-        <v>1.768</v>
+        <v>4.1479999999999997</v>
       </c>
       <c r="N65" s="10">
         <f t="shared" ref="N65" si="260">M65+N64</f>
-        <v>2.448</v>
+        <v>5.7799999999999994</v>
       </c>
       <c r="O65" s="10">
         <f t="shared" ref="O65" si="261">N65+O64</f>
-        <v>3.536</v>
+        <v>6.7999999999999989</v>
       </c>
       <c r="P65" s="10">
         <f t="shared" ref="P65" si="262">O65+P64</f>
-        <v>5.032</v>
+        <v>8.4319999999999986</v>
       </c>
       <c r="Q65" s="10">
         <f t="shared" ref="Q65" si="263">P65+Q64</f>
-        <v>6.5280000000000005</v>
+        <v>10.063999999999998</v>
       </c>
       <c r="R65" s="10">
         <f t="shared" ref="R65" si="264">Q65+R64</f>
-        <v>8.0240000000000009</v>
+        <v>11.695999999999998</v>
       </c>
       <c r="S65" s="10">
         <f t="shared" ref="S65" si="265">R65+S64</f>
-        <v>9.5200000000000014</v>
+        <v>13.327999999999998</v>
       </c>
       <c r="T65" s="10">
         <f t="shared" ref="T65" si="266">S65+T64</f>
-        <v>10.88</v>
+        <v>14.959999999999997</v>
       </c>
       <c r="U65" s="10">
         <f t="shared" ref="U65" si="267">T65+U64</f>
-        <v>10.88</v>
+        <v>15.299999999999997</v>
       </c>
       <c r="V65" s="10">
         <f t="shared" ref="V65" si="268">U65+V64</f>
-        <v>10.88</v>
+        <v>15.299999999999997</v>
       </c>
       <c r="W65" s="10">
         <f t="shared" ref="W65" si="269">V65+W64</f>
-        <v>10.88</v>
+        <v>15.299999999999997</v>
       </c>
       <c r="X65" s="10">
         <f t="shared" ref="X65" si="270">W65+X64</f>
-        <v>10.88</v>
+        <v>15.299999999999997</v>
       </c>
       <c r="Y65" s="10">
         <f t="shared" ref="Y65" si="271">X65+Y64</f>
-        <v>10.88</v>
+        <v>15.299999999999997</v>
       </c>
     </row>
     <row r="67" spans="2:27" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Stundenergänzt, Statusbericht 2 angefangen
</commit_message>
<xml_diff>
--- a/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
+++ b/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9647D7C0-B625-4E84-89FA-A4643C8654F9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F98FF2-72A0-44B4-AEEE-26A62D75E83B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten" sheetId="1" r:id="rId1"/>
@@ -4385,13 +4385,13 @@
                   <c:v>3.8079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4822,19 +4822,19 @@
                   <c:v>1.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.36</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6320000000000001</c:v>
+                  <c:v>2.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6687,31 +6687,31 @@
                   <c:v>3.8079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7178,37 +7178,37 @@
                   <c:v>1.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.36</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6320000000000001</c:v>
+                  <c:v>2.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9097,43 +9097,43 @@
                   <c:v>3.8079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.8079999999999998</c:v>
+                  <c:v>4.2839999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9624,49 +9624,49 @@
                   <c:v>1.36</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.36</c:v>
+                  <c:v>1.496</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.6320000000000001</c:v>
+                  <c:v>2.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3120000000000003</c:v>
+                  <c:v>4.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10648,11 +10648,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="10" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="M69" sqref="M69"/>
+      <selection pane="bottomRight" activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11233,8 +11233,12 @@
       <c r="L19" s="19">
         <v>2</v>
       </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19"/>
+      <c r="M19" s="19">
+        <v>3</v>
+      </c>
+      <c r="N19" s="19">
+        <v>0</v>
+      </c>
       <c r="O19" s="19"/>
       <c r="P19" s="19"/>
       <c r="Q19" s="19"/>
@@ -11248,7 +11252,7 @@
       <c r="Y19" s="19"/>
       <c r="AA19" s="22">
         <f>SUM(E19:Y19)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
@@ -11280,8 +11284,12 @@
       <c r="L20" s="19">
         <v>1</v>
       </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
+      <c r="M20" s="19">
+        <v>1</v>
+      </c>
+      <c r="N20" s="19">
+        <v>0</v>
+      </c>
       <c r="O20" s="19"/>
       <c r="P20" s="19"/>
       <c r="Q20" s="19"/>
@@ -11295,7 +11303,7 @@
       <c r="Y20" s="19"/>
       <c r="AA20" s="22">
         <f t="shared" ref="AA20:AA22" si="3">SUM(E20:Y20)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
@@ -11368,7 +11376,7 @@
       </c>
       <c r="M22" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="N22" s="20">
         <f t="shared" si="4"/>
@@ -11420,7 +11428,7 @@
       </c>
       <c r="AA22" s="20">
         <f t="shared" si="3"/>
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
@@ -11462,55 +11470,55 @@
       </c>
       <c r="M23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="N23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="O23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="P23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Q23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="R23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="S23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="T23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="U23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="V23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="W23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="X23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Y23" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AA23" s="5"/>
     </row>
@@ -11555,7 +11563,7 @@
       </c>
       <c r="M24" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="N24" s="10">
         <f t="shared" si="6"/>
@@ -11607,7 +11615,7 @@
       </c>
       <c r="AA24" s="10">
         <f>SUM(E24:Y24)</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
@@ -11654,55 +11662,55 @@
       </c>
       <c r="M25" s="10">
         <f t="shared" ref="M25" si="13">L25+M24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="N25" s="10">
         <f t="shared" ref="N25" si="14">M25+N24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="O25" s="10">
         <f t="shared" ref="O25" si="15">N25+O24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="P25" s="10">
         <f t="shared" ref="P25" si="16">O25+P24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="Q25" s="10">
         <f t="shared" ref="Q25" si="17">P25+Q24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="R25" s="10">
         <f t="shared" ref="R25" si="18">Q25+R24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="S25" s="10">
         <f t="shared" ref="S25" si="19">R25+S24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="T25" s="10">
         <f t="shared" ref="T25" si="20">S25+T24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="U25" s="10">
         <f t="shared" ref="U25" si="21">T25+U24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="V25" s="10">
         <f t="shared" ref="V25" si="22">U25+V24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="W25" s="10">
         <f t="shared" ref="W25" si="23">V25+W24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="X25" s="10">
         <f t="shared" ref="X25" si="24">W25+X24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
       <c r="Y25" s="10">
         <f t="shared" ref="Y25" si="25">X25+Y24</f>
-        <v>3.8079999999999998</v>
+        <v>4.2839999999999998</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
@@ -13956,8 +13964,12 @@
       <c r="I67" s="19"/>
       <c r="J67" s="19"/>
       <c r="K67" s="19"/>
-      <c r="L67" s="19"/>
-      <c r="M67" s="19"/>
+      <c r="L67" s="19">
+        <v>1</v>
+      </c>
+      <c r="M67" s="19">
+        <v>2</v>
+      </c>
       <c r="N67" s="19"/>
       <c r="O67" s="19"/>
       <c r="P67" s="19"/>
@@ -13972,7 +13984,7 @@
       <c r="Y67" s="19"/>
       <c r="AA67" s="22">
         <f>SUM(E67:Y67)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.25">
@@ -14032,9 +14044,15 @@
       </c>
       <c r="I69" s="19"/>
       <c r="J69" s="19"/>
-      <c r="K69" s="19"/>
-      <c r="L69" s="19"/>
-      <c r="M69" s="19"/>
+      <c r="K69" s="19">
+        <v>2</v>
+      </c>
+      <c r="L69" s="19">
+        <v>5</v>
+      </c>
+      <c r="M69" s="19">
+        <v>6</v>
+      </c>
       <c r="N69" s="19"/>
       <c r="O69" s="19"/>
       <c r="P69" s="19"/>
@@ -14064,8 +14082,12 @@
       <c r="I70" s="19"/>
       <c r="J70" s="19"/>
       <c r="K70" s="19"/>
-      <c r="L70" s="19"/>
-      <c r="M70" s="19"/>
+      <c r="L70" s="19">
+        <v>1</v>
+      </c>
+      <c r="M70" s="19">
+        <v>2</v>
+      </c>
       <c r="N70" s="19"/>
       <c r="O70" s="19"/>
       <c r="P70" s="19"/>
@@ -14094,8 +14116,12 @@
       <c r="I71" s="19"/>
       <c r="J71" s="19"/>
       <c r="K71" s="19"/>
-      <c r="L71" s="19"/>
-      <c r="M71" s="19"/>
+      <c r="L71" s="19">
+        <v>1</v>
+      </c>
+      <c r="M71" s="19">
+        <v>2</v>
+      </c>
       <c r="N71" s="19"/>
       <c r="O71" s="19"/>
       <c r="P71" s="19"/>
@@ -14110,7 +14136,7 @@
       <c r="Y71" s="19"/>
       <c r="AA71" s="22">
         <f t="shared" ref="AA71:AA73" si="260">SUM(E71:Y71)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.25">
@@ -14127,8 +14153,12 @@
       <c r="I72" s="19"/>
       <c r="J72" s="19"/>
       <c r="K72" s="19"/>
-      <c r="L72" s="19"/>
-      <c r="M72" s="19"/>
+      <c r="L72" s="19">
+        <v>1</v>
+      </c>
+      <c r="M72" s="19">
+        <v>3</v>
+      </c>
       <c r="N72" s="19"/>
       <c r="O72" s="19"/>
       <c r="P72" s="19"/>
@@ -14143,7 +14173,7 @@
       <c r="Y72" s="19"/>
       <c r="AA72" s="22">
         <f t="shared" si="260"/>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="2:27" x14ac:dyDescent="0.25">
@@ -14177,15 +14207,15 @@
       </c>
       <c r="K73" s="20">
         <f t="shared" ref="K73" si="266">SUM(K67:K72)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L73" s="20">
         <f t="shared" ref="L73" si="267">SUM(L67:L72)</f>
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="M73" s="20">
         <f t="shared" ref="M73" si="268">SUM(M67:M72)</f>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="N73" s="20">
         <f t="shared" ref="N73" si="269">SUM(N67:N72)</f>
@@ -14237,7 +14267,7 @@
       </c>
       <c r="AA73" s="20">
         <f t="shared" si="260"/>
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="74" spans="2:27" x14ac:dyDescent="0.25">
@@ -14271,63 +14301,63 @@
       </c>
       <c r="K74" s="18">
         <f t="shared" ref="K74" si="285">J74+K73</f>
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L74" s="18">
         <f t="shared" ref="L74" si="286">K74+L73</f>
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="M74" s="18">
         <f t="shared" ref="M74" si="287">L74+M73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="N74" s="18">
         <f t="shared" ref="N74" si="288">M74+N73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="O74" s="18">
         <f t="shared" ref="O74" si="289">N74+O73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="P74" s="18">
         <f t="shared" ref="P74" si="290">O74+P73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Q74" s="18">
         <f t="shared" ref="Q74" si="291">P74+Q73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="R74" s="18">
         <f t="shared" ref="R74" si="292">Q74+R73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="S74" s="18">
         <f t="shared" ref="S74" si="293">R74+S73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="T74" s="18">
         <f t="shared" ref="T74" si="294">S74+T73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="U74" s="18">
         <f t="shared" ref="U74" si="295">T74+U73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="V74" s="18">
         <f t="shared" ref="V74" si="296">U74+V73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="W74" s="18">
         <f t="shared" ref="W74" si="297">V74+W73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="X74" s="18">
         <f t="shared" ref="X74" si="298">W74+X73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="Y74" s="18">
         <f t="shared" ref="Y74" si="299">X74+Y73</f>
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="AA74" s="5"/>
     </row>
@@ -14364,15 +14394,15 @@
       </c>
       <c r="K75" s="10">
         <f t="shared" si="300"/>
-        <v>0</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="L75" s="10">
         <f t="shared" si="300"/>
-        <v>0.27200000000000002</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="M75" s="10">
         <f t="shared" si="300"/>
-        <v>0.68</v>
+        <v>1.7</v>
       </c>
       <c r="N75" s="10">
         <f t="shared" si="300"/>
@@ -14424,7 +14454,7 @@
       </c>
       <c r="AA75" s="10">
         <f>SUM(E75:Y75)</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.25">
@@ -14463,63 +14493,63 @@
       </c>
       <c r="K76" s="10">
         <f t="shared" ref="K76" si="305">J76+K75</f>
-        <v>1.36</v>
+        <v>1.496</v>
       </c>
       <c r="L76" s="10">
         <f t="shared" ref="L76" si="306">K76+L75</f>
-        <v>1.6320000000000001</v>
+        <v>2.38</v>
       </c>
       <c r="M76" s="10">
         <f t="shared" ref="M76" si="307">L76+M75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="N76" s="10">
         <f t="shared" ref="N76" si="308">M76+N75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="O76" s="10">
         <f t="shared" ref="O76" si="309">N76+O75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="P76" s="10">
         <f t="shared" ref="P76" si="310">O76+P75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="Q76" s="10">
         <f t="shared" ref="Q76" si="311">P76+Q75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="R76" s="10">
         <f t="shared" ref="R76" si="312">Q76+R75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="S76" s="10">
         <f t="shared" ref="S76" si="313">R76+S75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="T76" s="10">
         <f t="shared" ref="T76" si="314">S76+T75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="U76" s="10">
         <f t="shared" ref="U76" si="315">T76+U75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="V76" s="10">
         <f t="shared" ref="V76" si="316">U76+V75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="W76" s="10">
         <f t="shared" ref="W76" si="317">V76+W75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="X76" s="10">
         <f t="shared" ref="X76" si="318">W76+X75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
       <c r="Y76" s="10">
         <f t="shared" ref="Y76" si="319">X76+Y75</f>
-        <v>2.3120000000000003</v>
+        <v>4.08</v>
       </c>
     </row>
     <row r="79" spans="2:27" x14ac:dyDescent="0.25">
@@ -16366,7 +16396,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
statusbericht stunden eingetragen und to do notizen von dalessandro
</commit_message>
<xml_diff>
--- a/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
+++ b/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D2A13C-F71B-448D-9E19-BE6D0ADB3F1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390BD31E-21ED-4C78-8831-9456F8D54F72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="13800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten" sheetId="1" r:id="rId1"/>
@@ -7198,16 +7198,16 @@
                   <c:v>16.184000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.788</c:v>
+                  <c:v>20.128</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.14</c:v>
+                  <c:v>24.48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7295,10 +7295,10 @@
                   <c:v>2.1759999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9644,28 +9644,28 @@
                   <c:v>16.184000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19.788</c:v>
+                  <c:v>20.128</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.14</c:v>
+                  <c:v>24.48</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24.14</c:v>
+                  <c:v>27.132000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9753,22 +9753,22 @@
                   <c:v>2.1759999999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.1759999999999997</c:v>
+                  <c:v>4.0119999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10647,11 +10647,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA112"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="10" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="R69" sqref="R69"/>
+      <selection pane="bottomRight" activeCell="T73" sqref="T73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13982,12 +13982,14 @@
         <v>9</v>
       </c>
       <c r="R67" s="19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S67" s="19">
         <v>10</v>
       </c>
-      <c r="T67" s="19"/>
+      <c r="T67" s="19">
+        <v>9</v>
+      </c>
       <c r="U67" s="19"/>
       <c r="V67" s="19"/>
       <c r="W67" s="19"/>
@@ -13995,7 +13997,7 @@
       <c r="Y67" s="19"/>
       <c r="AA67" s="22">
         <f>SUM(E67:Y67)</f>
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.25">
@@ -14043,7 +14045,9 @@
       <c r="S68" s="19">
         <v>15</v>
       </c>
-      <c r="T68" s="19"/>
+      <c r="T68" s="19">
+        <v>10</v>
+      </c>
       <c r="U68" s="19"/>
       <c r="V68" s="19"/>
       <c r="W68" s="19"/>
@@ -14089,12 +14093,14 @@
         <v>9</v>
       </c>
       <c r="R69" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S69" s="19">
         <v>9</v>
       </c>
-      <c r="T69" s="19"/>
+      <c r="T69" s="19">
+        <v>1</v>
+      </c>
       <c r="U69" s="19"/>
       <c r="V69" s="19"/>
       <c r="W69" s="19"/>
@@ -14136,12 +14142,14 @@
         <v>9</v>
       </c>
       <c r="R70" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S70" s="19">
         <v>12</v>
       </c>
-      <c r="T70" s="19"/>
+      <c r="T70" s="19">
+        <v>9</v>
+      </c>
       <c r="U70" s="19"/>
       <c r="V70" s="19"/>
       <c r="W70" s="19"/>
@@ -14182,12 +14190,14 @@
         <v>9</v>
       </c>
       <c r="R71" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S71" s="19">
         <v>9</v>
       </c>
-      <c r="T71" s="19"/>
+      <c r="T71" s="19">
+        <v>1</v>
+      </c>
       <c r="U71" s="19"/>
       <c r="V71" s="19"/>
       <c r="W71" s="19"/>
@@ -14195,7 +14205,7 @@
       <c r="Y71" s="19"/>
       <c r="AA71" s="22">
         <f t="shared" ref="AA71:AA73" si="260">SUM(E71:Y71)</f>
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.25">
@@ -14231,12 +14241,14 @@
         <v>9</v>
       </c>
       <c r="R72" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S72" s="19">
         <v>9</v>
       </c>
-      <c r="T72" s="19"/>
+      <c r="T72" s="19">
+        <v>9</v>
+      </c>
       <c r="U72" s="19"/>
       <c r="V72" s="19"/>
       <c r="W72" s="19"/>
@@ -14244,7 +14256,7 @@
       <c r="Y72" s="19"/>
       <c r="AA72" s="22">
         <f t="shared" si="260"/>
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="73" spans="2:27" x14ac:dyDescent="0.25">
@@ -14306,7 +14318,7 @@
       </c>
       <c r="R73" s="20">
         <f t="shared" ref="R73" si="273">SUM(R67:R72)</f>
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="S73" s="20">
         <f t="shared" ref="S73" si="274">SUM(S67:S72)</f>
@@ -14314,7 +14326,7 @@
       </c>
       <c r="T73" s="20">
         <f t="shared" ref="T73" si="275">SUM(T67:T72)</f>
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="U73" s="20">
         <f t="shared" ref="U73" si="276">SUM(U67:U72)</f>
@@ -14338,7 +14350,7 @@
       </c>
       <c r="AA73" s="20">
         <f t="shared" si="260"/>
-        <v>355</v>
+        <v>399</v>
       </c>
     </row>
     <row r="74" spans="2:27" x14ac:dyDescent="0.25">
@@ -14400,35 +14412,35 @@
       </c>
       <c r="R74" s="18">
         <f t="shared" ref="R74" si="292">Q74+R73</f>
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="S74" s="18">
         <f t="shared" ref="S74" si="293">R74+S73</f>
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="T74" s="18">
         <f t="shared" ref="T74" si="294">S74+T73</f>
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="U74" s="18">
         <f t="shared" ref="U74" si="295">T74+U73</f>
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="V74" s="18">
         <f t="shared" ref="V74" si="296">U74+V73</f>
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="W74" s="18">
         <f t="shared" ref="W74" si="297">V74+W73</f>
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="X74" s="18">
         <f t="shared" ref="X74" si="298">W74+X73</f>
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="Y74" s="18">
         <f t="shared" ref="Y74" si="299">X74+Y73</f>
-        <v>355</v>
+        <v>399</v>
       </c>
       <c r="AA74" s="5"/>
     </row>
@@ -14493,7 +14505,7 @@
       </c>
       <c r="R75" s="10">
         <f t="shared" si="300"/>
-        <v>3.6040000000000001</v>
+        <v>3.944</v>
       </c>
       <c r="S75" s="10">
         <f t="shared" si="300"/>
@@ -14501,7 +14513,7 @@
       </c>
       <c r="T75" s="10">
         <f t="shared" si="300"/>
-        <v>0</v>
+        <v>2.6520000000000001</v>
       </c>
       <c r="U75" s="10">
         <f t="shared" si="300"/>
@@ -14525,7 +14537,7 @@
       </c>
       <c r="AA75" s="10">
         <f>SUM(E75:Y75)</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.25">
@@ -14592,35 +14604,35 @@
       </c>
       <c r="R76" s="10">
         <f t="shared" ref="R76" si="312">Q76+R75</f>
-        <v>19.788</v>
+        <v>20.128</v>
       </c>
       <c r="S76" s="10">
         <f t="shared" ref="S76" si="313">R76+S75</f>
-        <v>24.14</v>
+        <v>24.48</v>
       </c>
       <c r="T76" s="10">
         <f t="shared" ref="T76" si="314">S76+T75</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
       <c r="U76" s="10">
         <f t="shared" ref="U76" si="315">T76+U75</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
       <c r="V76" s="10">
         <f t="shared" ref="V76" si="316">U76+V75</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
       <c r="W76" s="10">
         <f t="shared" ref="W76" si="317">V76+W75</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
       <c r="X76" s="10">
         <f t="shared" ref="X76" si="318">W76+X75</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
       <c r="Y76" s="10">
         <f t="shared" ref="Y76" si="319">X76+Y75</f>
-        <v>24.14</v>
+        <v>27.132000000000001</v>
       </c>
     </row>
     <row r="79" spans="2:27" x14ac:dyDescent="0.25">
@@ -15050,7 +15062,9 @@
       <c r="S86" s="19">
         <v>1</v>
       </c>
-      <c r="T86" s="19"/>
+      <c r="T86" s="19">
+        <v>9</v>
+      </c>
       <c r="U86" s="19"/>
       <c r="V86" s="19"/>
       <c r="W86" s="19"/>
@@ -15093,7 +15107,9 @@
       <c r="S87" s="19">
         <v>1</v>
       </c>
-      <c r="T87" s="19"/>
+      <c r="T87" s="19">
+        <v>9</v>
+      </c>
       <c r="U87" s="19"/>
       <c r="V87" s="19"/>
       <c r="W87" s="19"/>
@@ -15174,7 +15190,9 @@
       <c r="S89" s="19">
         <v>1</v>
       </c>
-      <c r="T89" s="19"/>
+      <c r="T89" s="19">
+        <v>9</v>
+      </c>
       <c r="U89" s="19"/>
       <c r="V89" s="19"/>
       <c r="W89" s="19"/>
@@ -15182,7 +15200,7 @@
       <c r="Y89" s="19"/>
       <c r="AA89" s="22">
         <f t="shared" ref="AA89:AA91" si="358">SUM(E89:Y89)</f>
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="2:27" x14ac:dyDescent="0.25">
@@ -15295,7 +15313,7 @@
       </c>
       <c r="T91" s="20">
         <f t="shared" ref="T91" si="373">SUM(T85:T90)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="U91" s="20">
         <f t="shared" ref="U91" si="374">SUM(U85:U90)</f>
@@ -15319,7 +15337,7 @@
       </c>
       <c r="AA91" s="20">
         <f t="shared" si="358"/>
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
     <row r="92" spans="2:27" x14ac:dyDescent="0.25">
@@ -15389,27 +15407,27 @@
       </c>
       <c r="T92" s="18">
         <f t="shared" ref="T92" si="392">S92+T91</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="U92" s="18">
         <f t="shared" ref="U92" si="393">T92+U91</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="V92" s="18">
         <f t="shared" ref="V92" si="394">U92+V91</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="W92" s="18">
         <f t="shared" ref="W92" si="395">V92+W91</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="X92" s="18">
         <f t="shared" ref="X92" si="396">W92+X91</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="Y92" s="18">
         <f t="shared" ref="Y92" si="397">X92+Y91</f>
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="AA92" s="5"/>
     </row>
@@ -15482,7 +15500,7 @@
       </c>
       <c r="T93" s="10">
         <f t="shared" si="398"/>
-        <v>0</v>
+        <v>1.8360000000000001</v>
       </c>
       <c r="U93" s="10">
         <f t="shared" si="398"/>
@@ -15506,7 +15524,7 @@
       </c>
       <c r="AA93" s="10">
         <f>SUM(E93:Y93)</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:27" x14ac:dyDescent="0.25">
@@ -15581,27 +15599,27 @@
       </c>
       <c r="T94" s="10">
         <f t="shared" ref="T94" si="412">S94+T93</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="U94" s="10">
         <f t="shared" ref="U94" si="413">T94+U93</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="V94" s="10">
         <f t="shared" ref="V94" si="414">U94+V93</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="W94" s="10">
         <f t="shared" ref="W94" si="415">V94+W93</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="X94" s="10">
         <f t="shared" ref="X94" si="416">W94+X93</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
       <c r="Y94" s="10">
         <f t="shared" ref="Y94" si="417">X94+Y93</f>
-        <v>2.1759999999999997</v>
+        <v>4.0119999999999996</v>
       </c>
     </row>
     <row r="97" spans="2:27" x14ac:dyDescent="0.25">
@@ -16552,7 +16570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
@@ -16567,7 +16585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bisschen am statusbericht 4 gschaffelet
</commit_message>
<xml_diff>
--- a/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
+++ b/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564C06AD-DA63-4362-B1E0-95E0A77822F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1279D7-5057-4942-A336-57659594FDDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9123,16 +9123,16 @@
                   <c:v>5.4144999999999994</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4144999999999994</c:v>
+                  <c:v>5.7714999999999996</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.4144999999999994</c:v>
+                  <c:v>6.2474999999999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.4144999999999994</c:v>
+                  <c:v>6.7234999999999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.4144999999999994</c:v>
+                  <c:v>6.7234999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9656,16 +9656,16 @@
                   <c:v>28.900000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.716000000000001</c:v>
+                  <c:v>30.94</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.396000000000001</c:v>
+                  <c:v>32.707999999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>31.076000000000001</c:v>
+                  <c:v>34.747999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31.756</c:v>
+                  <c:v>35.088000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9759,16 +9759,16 @@
                   <c:v>5.7119999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.7119999999999997</c:v>
+                  <c:v>6.7319999999999993</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.7119999999999997</c:v>
+                  <c:v>7.4799999999999995</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.7119999999999997</c:v>
+                  <c:v>8.0919999999999987</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.7119999999999997</c:v>
+                  <c:v>8.2959999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9868,10 +9868,10 @@
                   <c:v>0.47599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.47599999999999998</c:v>
+                  <c:v>0.8839999999999999</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.47599999999999998</c:v>
+                  <c:v>1.6999999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10648,10 +10648,10 @@
   <dimension ref="B2:AA112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="10" topLeftCell="E101" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="X67" sqref="X67"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11259,13 +11259,19 @@
       <c r="U19" s="19">
         <v>4</v>
       </c>
-      <c r="V19" s="19"/>
-      <c r="W19" s="19"/>
-      <c r="X19" s="19"/>
+      <c r="V19" s="19">
+        <v>2</v>
+      </c>
+      <c r="W19" s="19">
+        <v>3</v>
+      </c>
+      <c r="X19" s="19">
+        <v>3</v>
+      </c>
       <c r="Y19" s="19"/>
       <c r="AA19" s="22">
         <f>SUM(E19:Y19)</f>
-        <v>31.5</v>
+        <v>39.5</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
@@ -11312,13 +11318,19 @@
       <c r="U20" s="19">
         <v>1</v>
       </c>
-      <c r="V20" s="19"/>
-      <c r="W20" s="19"/>
-      <c r="X20" s="19"/>
+      <c r="V20" s="19">
+        <v>1</v>
+      </c>
+      <c r="W20" s="19">
+        <v>1</v>
+      </c>
+      <c r="X20" s="19">
+        <v>1</v>
+      </c>
       <c r="Y20" s="19"/>
       <c r="AA20" s="22">
         <f t="shared" ref="AA20:AA22" si="3">SUM(E20:Y20)</f>
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:27" x14ac:dyDescent="0.25">
@@ -11427,15 +11439,15 @@
       </c>
       <c r="V22" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W22" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X22" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y22" s="20">
         <f t="shared" si="4"/>
@@ -11443,7 +11455,7 @@
       </c>
       <c r="AA22" s="20">
         <f t="shared" si="3"/>
-        <v>45.5</v>
+        <v>56.5</v>
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
@@ -11521,19 +11533,19 @@
       </c>
       <c r="V23" s="18">
         <f t="shared" si="5"/>
-        <v>43.5</v>
+        <v>46.5</v>
       </c>
       <c r="W23" s="18">
         <f t="shared" si="5"/>
-        <v>43.5</v>
+        <v>50.5</v>
       </c>
       <c r="X23" s="18">
         <f t="shared" si="5"/>
-        <v>43.5</v>
+        <v>54.5</v>
       </c>
       <c r="Y23" s="18">
         <f t="shared" si="5"/>
-        <v>43.5</v>
+        <v>54.5</v>
       </c>
       <c r="AA23" s="5"/>
     </row>
@@ -11614,15 +11626,15 @@
       </c>
       <c r="V24" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="W24" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="X24" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="Y24" s="10">
         <f t="shared" si="6"/>
@@ -11630,7 +11642,7 @@
       </c>
       <c r="AA24" s="10">
         <f>SUM(E24:Y24)</f>
-        <v>5.4144999999999994</v>
+        <v>6.7234999999999996</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
@@ -11713,19 +11725,19 @@
       </c>
       <c r="V25" s="10">
         <f t="shared" ref="V25" si="22">U25+V24</f>
-        <v>5.4144999999999994</v>
+        <v>5.7714999999999996</v>
       </c>
       <c r="W25" s="10">
         <f t="shared" ref="W25" si="23">V25+W24</f>
-        <v>5.4144999999999994</v>
+        <v>6.2474999999999996</v>
       </c>
       <c r="X25" s="10">
         <f t="shared" ref="X25" si="24">W25+X24</f>
-        <v>5.4144999999999994</v>
+        <v>6.7234999999999996</v>
       </c>
       <c r="Y25" s="10">
         <f t="shared" ref="Y25" si="25">X25+Y24</f>
-        <v>5.4144999999999994</v>
+        <v>6.7234999999999996</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
@@ -14013,11 +14025,13 @@
         <v>2</v>
       </c>
       <c r="W67" s="19"/>
-      <c r="X67" s="19"/>
+      <c r="X67" s="19">
+        <v>2</v>
+      </c>
       <c r="Y67" s="19"/>
       <c r="AA67" s="22">
         <f>SUM(E67:Y67)</f>
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.25">
@@ -14078,10 +14092,10 @@
         <v>10</v>
       </c>
       <c r="X68" s="19">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="Y68" s="19">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AA68" s="22"/>
     </row>
@@ -14134,9 +14148,15 @@
       <c r="U69" s="19">
         <v>5</v>
       </c>
-      <c r="V69" s="19"/>
-      <c r="W69" s="19"/>
-      <c r="X69" s="19"/>
+      <c r="V69" s="19">
+        <v>8</v>
+      </c>
+      <c r="W69" s="19">
+        <v>5</v>
+      </c>
+      <c r="X69" s="19">
+        <v>5</v>
+      </c>
       <c r="Y69" s="19"/>
       <c r="AA69" s="22"/>
     </row>
@@ -14185,9 +14205,15 @@
       <c r="U70" s="19">
         <v>3</v>
       </c>
-      <c r="V70" s="19"/>
-      <c r="W70" s="19"/>
-      <c r="X70" s="19"/>
+      <c r="V70" s="19">
+        <v>5</v>
+      </c>
+      <c r="W70" s="19">
+        <v>2</v>
+      </c>
+      <c r="X70" s="19">
+        <v>2</v>
+      </c>
       <c r="Y70" s="19"/>
       <c r="AA70" s="22"/>
     </row>
@@ -14235,13 +14261,19 @@
       <c r="U71" s="19">
         <v>3</v>
       </c>
-      <c r="V71" s="19"/>
-      <c r="W71" s="19"/>
-      <c r="X71" s="19"/>
+      <c r="V71" s="19">
+        <v>5</v>
+      </c>
+      <c r="W71" s="19">
+        <v>8</v>
+      </c>
+      <c r="X71" s="19">
+        <v>5</v>
+      </c>
       <c r="Y71" s="19"/>
       <c r="AA71" s="22">
         <f t="shared" ref="AA71:AA73" si="260">SUM(E71:Y71)</f>
-        <v>54</v>
+        <v>72</v>
       </c>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.25">
@@ -14289,12 +14321,16 @@
         <v>3</v>
       </c>
       <c r="V72" s="19"/>
-      <c r="W72" s="19"/>
-      <c r="X72" s="19"/>
+      <c r="W72" s="19">
+        <v>1</v>
+      </c>
+      <c r="X72" s="19">
+        <v>1</v>
+      </c>
       <c r="Y72" s="19"/>
       <c r="AA72" s="22">
         <f t="shared" si="260"/>
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="73" spans="2:27" x14ac:dyDescent="0.25">
@@ -14372,23 +14408,23 @@
       </c>
       <c r="V73" s="20">
         <f t="shared" ref="V73" si="277">SUM(V67:V72)</f>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="W73" s="20">
         <f t="shared" ref="W73" si="278">SUM(W67:W72)</f>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="X73" s="20">
         <f t="shared" ref="X73" si="279">SUM(X67:X72)</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="Y73" s="20">
         <f t="shared" ref="Y73" si="280">SUM(Y67:Y72)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="AA73" s="20">
         <f t="shared" si="260"/>
-        <v>467</v>
+        <v>516</v>
       </c>
     </row>
     <row r="74" spans="2:27" x14ac:dyDescent="0.25">
@@ -14466,19 +14502,19 @@
       </c>
       <c r="V74" s="18">
         <f t="shared" ref="V74" si="296">U74+V73</f>
-        <v>437</v>
+        <v>455</v>
       </c>
       <c r="W74" s="18">
         <f t="shared" ref="W74" si="297">V74+W73</f>
-        <v>447</v>
+        <v>481</v>
       </c>
       <c r="X74" s="18">
         <f t="shared" ref="X74" si="298">W74+X73</f>
-        <v>457</v>
+        <v>511</v>
       </c>
       <c r="Y74" s="18">
         <f t="shared" ref="Y74" si="299">X74+Y73</f>
-        <v>467</v>
+        <v>516</v>
       </c>
       <c r="AA74" s="5"/>
     </row>
@@ -14559,23 +14595,23 @@
       </c>
       <c r="V75" s="10">
         <f t="shared" si="300"/>
-        <v>0.81599999999999995</v>
+        <v>2.04</v>
       </c>
       <c r="W75" s="10">
         <f t="shared" si="300"/>
-        <v>0.68</v>
+        <v>1.768</v>
       </c>
       <c r="X75" s="10">
         <f t="shared" si="300"/>
-        <v>0.68</v>
+        <v>2.04</v>
       </c>
       <c r="Y75" s="10">
         <f t="shared" si="300"/>
-        <v>0.68</v>
+        <v>0.34</v>
       </c>
       <c r="AA75" s="10">
         <f>SUM(E75:Y75)</f>
-        <v>31.756</v>
+        <v>35.088000000000001</v>
       </c>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.25">
@@ -14658,19 +14694,19 @@
       </c>
       <c r="V76" s="10">
         <f t="shared" ref="V76" si="316">U76+V75</f>
-        <v>29.716000000000001</v>
+        <v>30.94</v>
       </c>
       <c r="W76" s="10">
         <f t="shared" ref="W76" si="317">V76+W75</f>
-        <v>30.396000000000001</v>
+        <v>32.707999999999998</v>
       </c>
       <c r="X76" s="10">
         <f t="shared" ref="X76" si="318">W76+X75</f>
-        <v>31.076000000000001</v>
+        <v>34.747999999999998</v>
       </c>
       <c r="Y76" s="10">
         <f t="shared" ref="Y76" si="319">X76+Y75</f>
-        <v>31.756</v>
+        <v>35.088000000000001</v>
       </c>
     </row>
     <row r="79" spans="2:27" x14ac:dyDescent="0.25">
@@ -15058,13 +15094,21 @@
       <c r="U85" s="19">
         <v>5</v>
       </c>
-      <c r="V85" s="19"/>
-      <c r="W85" s="19"/>
-      <c r="X85" s="19"/>
-      <c r="Y85" s="19"/>
+      <c r="V85" s="19">
+        <v>3</v>
+      </c>
+      <c r="W85" s="19">
+        <v>3</v>
+      </c>
+      <c r="X85" s="19">
+        <v>3</v>
+      </c>
+      <c r="Y85" s="19">
+        <v>3</v>
+      </c>
       <c r="AA85" s="22">
         <f>SUM(E85:Y85)</f>
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="2:27" x14ac:dyDescent="0.25">
@@ -15153,9 +15197,15 @@
       <c r="U87" s="19">
         <v>5</v>
       </c>
-      <c r="V87" s="19"/>
-      <c r="W87" s="19"/>
-      <c r="X87" s="19"/>
+      <c r="V87" s="19">
+        <v>5</v>
+      </c>
+      <c r="W87" s="19">
+        <v>5</v>
+      </c>
+      <c r="X87" s="19">
+        <v>5</v>
+      </c>
       <c r="Y87" s="19"/>
       <c r="AA87" s="22"/>
     </row>
@@ -15196,8 +15246,12 @@
       <c r="U88" s="19">
         <v>5</v>
       </c>
-      <c r="V88" s="19"/>
-      <c r="W88" s="19"/>
+      <c r="V88" s="19">
+        <v>2</v>
+      </c>
+      <c r="W88" s="19">
+        <v>2</v>
+      </c>
       <c r="X88" s="19"/>
       <c r="Y88" s="19"/>
       <c r="AA88" s="22"/>
@@ -15240,13 +15294,19 @@
       <c r="U89" s="19">
         <v>5</v>
       </c>
-      <c r="V89" s="19"/>
-      <c r="W89" s="19"/>
-      <c r="X89" s="19"/>
+      <c r="V89" s="19">
+        <v>5</v>
+      </c>
+      <c r="W89" s="19">
+        <v>1</v>
+      </c>
+      <c r="X89" s="19">
+        <v>1</v>
+      </c>
       <c r="Y89" s="19"/>
       <c r="AA89" s="22">
         <f t="shared" ref="AA89:AA91" si="358">SUM(E89:Y89)</f>
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="90" spans="2:27" x14ac:dyDescent="0.25">
@@ -15369,23 +15429,23 @@
       </c>
       <c r="V91" s="20">
         <f t="shared" ref="V91" si="375">SUM(V85:V90)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="W91" s="20">
         <f t="shared" ref="W91" si="376">SUM(W85:W90)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="X91" s="20">
         <f t="shared" ref="X91" si="377">SUM(X85:X90)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Y91" s="20">
         <f t="shared" ref="Y91" si="378">SUM(Y85:Y90)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AA91" s="20">
         <f t="shared" si="358"/>
-        <v>84</v>
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="2:27" x14ac:dyDescent="0.25">
@@ -15463,19 +15523,19 @@
       </c>
       <c r="V92" s="18">
         <f t="shared" ref="V92" si="394">U92+V91</f>
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="W92" s="18">
         <f t="shared" ref="W92" si="395">V92+W91</f>
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="X92" s="18">
         <f t="shared" ref="X92" si="396">W92+X91</f>
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="Y92" s="18">
         <f t="shared" ref="Y92" si="397">X92+Y91</f>
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="AA92" s="5"/>
     </row>
@@ -15556,23 +15616,23 @@
       </c>
       <c r="V93" s="10">
         <f t="shared" si="398"/>
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="W93" s="10">
         <f t="shared" si="398"/>
-        <v>0</v>
+        <v>0.748</v>
       </c>
       <c r="X93" s="10">
         <f t="shared" si="398"/>
-        <v>0</v>
+        <v>0.61199999999999999</v>
       </c>
       <c r="Y93" s="10">
         <f t="shared" si="398"/>
-        <v>0</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="AA93" s="10">
         <f>SUM(E93:Y93)</f>
-        <v>5.7119999999999997</v>
+        <v>8.2959999999999994</v>
       </c>
     </row>
     <row r="94" spans="2:27" x14ac:dyDescent="0.25">
@@ -15655,19 +15715,19 @@
       </c>
       <c r="V94" s="10">
         <f t="shared" ref="V94" si="414">U94+V93</f>
-        <v>5.7119999999999997</v>
+        <v>6.7319999999999993</v>
       </c>
       <c r="W94" s="10">
         <f t="shared" ref="W94" si="415">V94+W93</f>
-        <v>5.7119999999999997</v>
+        <v>7.4799999999999995</v>
       </c>
       <c r="X94" s="10">
         <f t="shared" ref="X94" si="416">W94+X93</f>
-        <v>5.7119999999999997</v>
+        <v>8.0919999999999987</v>
       </c>
       <c r="Y94" s="10">
         <f t="shared" ref="Y94" si="417">X94+Y93</f>
-        <v>5.7119999999999997</v>
+        <v>8.2959999999999994</v>
       </c>
     </row>
     <row r="97" spans="2:27" x14ac:dyDescent="0.25">
@@ -16029,11 +16089,15 @@
       <c r="U103" s="19"/>
       <c r="V103" s="19"/>
       <c r="W103" s="19"/>
-      <c r="X103" s="19"/>
-      <c r="Y103" s="19"/>
+      <c r="X103" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y103" s="19">
+        <v>4</v>
+      </c>
       <c r="AA103" s="22">
         <f>SUM(E103:Y103)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104" spans="2:27" x14ac:dyDescent="0.25">
@@ -16063,8 +16127,12 @@
       <c r="U104" s="19"/>
       <c r="V104" s="19"/>
       <c r="W104" s="19"/>
-      <c r="X104" s="19"/>
-      <c r="Y104" s="19"/>
+      <c r="X104" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y104" s="19">
+        <v>4</v>
+      </c>
       <c r="AA104" s="22"/>
     </row>
     <row r="105" spans="2:27" x14ac:dyDescent="0.25">
@@ -16094,8 +16162,12 @@
       <c r="U105" s="19"/>
       <c r="V105" s="19"/>
       <c r="W105" s="19"/>
-      <c r="X105" s="19"/>
-      <c r="Y105" s="19"/>
+      <c r="X105" s="19">
+        <v>2</v>
+      </c>
+      <c r="Y105" s="19">
+        <v>4</v>
+      </c>
       <c r="AA105" s="22"/>
     </row>
     <row r="106" spans="2:27" x14ac:dyDescent="0.25">
@@ -16284,15 +16356,15 @@
       </c>
       <c r="X109" s="20">
         <f t="shared" ref="X109" si="475">SUM(X103:X108)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y109" s="20">
         <f t="shared" ref="Y109" si="476">SUM(Y103:Y108)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="AA109" s="20">
         <f t="shared" si="456"/>
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="110" spans="2:27" x14ac:dyDescent="0.25">
@@ -16378,11 +16450,11 @@
       </c>
       <c r="X110" s="18">
         <f t="shared" ref="X110" si="494">W110+X109</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="Y110" s="18">
         <f t="shared" ref="Y110" si="495">X110+Y109</f>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="AA110" s="5"/>
     </row>
@@ -16471,15 +16543,15 @@
       </c>
       <c r="X111" s="10">
         <f t="shared" si="496"/>
-        <v>0</v>
+        <v>0.40799999999999997</v>
       </c>
       <c r="Y111" s="10">
         <f t="shared" si="496"/>
-        <v>0</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="AA111" s="10">
         <f>SUM(E111:Y111)</f>
-        <v>0.47599999999999998</v>
+        <v>1.6999999999999997</v>
       </c>
     </row>
     <row r="112" spans="2:27" x14ac:dyDescent="0.25">
@@ -16570,11 +16642,11 @@
       </c>
       <c r="X112" s="10">
         <f t="shared" ref="X112" si="514">W112+X111</f>
-        <v>0.47599999999999998</v>
+        <v>0.8839999999999999</v>
       </c>
       <c r="Y112" s="10">
         <f t="shared" ref="Y112" si="515">X112+Y111</f>
-        <v>0.47599999999999998</v>
+        <v>1.6999999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -16635,7 +16707,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
versucht fertigzustellen aber nein
</commit_message>
<xml_diff>
--- a/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
+++ b/Statusberichte/19FS_pro2E_Team_5_Personalkosten_Tracking.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D1279D7-5057-4942-A336-57659594FDDD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B33985A-0F59-4239-AFD6-F41741CA51A8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="141">
   <si>
     <t>Plan</t>
   </si>
@@ -447,6 +447,12 @@
   <si>
     <t>Risiko-faktor</t>
   </si>
+  <si>
+    <t>Total Plan</t>
+  </si>
+  <si>
+    <t>Total Real</t>
+  </si>
 </sst>
 </file>
 
@@ -9132,7 +9138,7 @@
                   <c:v>6.7234999999999996</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.7234999999999996</c:v>
+                  <c:v>7.1994999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9662,10 +9668,10 @@
                   <c:v>32.707999999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>34.747999999999998</c:v>
+                  <c:v>34.951999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35.088000000000001</c:v>
+                  <c:v>37.128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9759,16 +9765,16 @@
                   <c:v>5.7119999999999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.7319999999999993</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.4799999999999995</c:v>
+                  <c:v>7.6159999999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.0919999999999987</c:v>
+                  <c:v>8.2959999999999994</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.2959999999999994</c:v>
+                  <c:v>9.3159999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10645,13 +10651,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:AA112"/>
+  <dimension ref="B2:AA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="10" topLeftCell="E101" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="10" topLeftCell="E88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C43" sqref="C43"/>
+      <selection pane="bottomRight" activeCell="Y117" sqref="Y117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11268,10 +11274,12 @@
       <c r="X19" s="19">
         <v>3</v>
       </c>
-      <c r="Y19" s="19"/>
+      <c r="Y19" s="19">
+        <v>4</v>
+      </c>
       <c r="AA19" s="22">
         <f>SUM(E19:Y19)</f>
-        <v>39.5</v>
+        <v>43.5</v>
       </c>
     </row>
     <row r="20" spans="2:27" x14ac:dyDescent="0.25">
@@ -11327,7 +11335,9 @@
       <c r="X20" s="19">
         <v>1</v>
       </c>
-      <c r="Y20" s="19"/>
+      <c r="Y20" s="19">
+        <v>0</v>
+      </c>
       <c r="AA20" s="22">
         <f t="shared" ref="AA20:AA22" si="3">SUM(E20:Y20)</f>
         <v>17</v>
@@ -11451,11 +11461,11 @@
       </c>
       <c r="Y22" s="20">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AA22" s="20">
         <f t="shared" si="3"/>
-        <v>56.5</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="23" spans="2:27" x14ac:dyDescent="0.25">
@@ -11545,7 +11555,7 @@
       </c>
       <c r="Y23" s="18">
         <f t="shared" si="5"/>
-        <v>54.5</v>
+        <v>58.5</v>
       </c>
       <c r="AA23" s="5"/>
     </row>
@@ -11638,11 +11648,11 @@
       </c>
       <c r="Y24" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="AA24" s="10">
         <f>SUM(E24:Y24)</f>
-        <v>6.7234999999999996</v>
+        <v>7.1994999999999996</v>
       </c>
     </row>
     <row r="25" spans="2:27" x14ac:dyDescent="0.25">
@@ -11737,7 +11747,7 @@
       </c>
       <c r="Y25" s="10">
         <f t="shared" ref="Y25" si="25">X25+Y24</f>
-        <v>6.7234999999999996</v>
+        <v>7.1994999999999996</v>
       </c>
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
@@ -14028,10 +14038,12 @@
       <c r="X67" s="19">
         <v>2</v>
       </c>
-      <c r="Y67" s="19"/>
+      <c r="Y67" s="19">
+        <v>3</v>
+      </c>
       <c r="AA67" s="22">
         <f>SUM(E67:Y67)</f>
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="2:27" x14ac:dyDescent="0.25">
@@ -14095,7 +14107,7 @@
         <v>15</v>
       </c>
       <c r="Y68" s="19">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AA68" s="22"/>
     </row>
@@ -14157,7 +14169,9 @@
       <c r="X69" s="19">
         <v>5</v>
       </c>
-      <c r="Y69" s="19"/>
+      <c r="Y69" s="19">
+        <v>8</v>
+      </c>
       <c r="AA69" s="22"/>
     </row>
     <row r="70" spans="2:27" x14ac:dyDescent="0.25">
@@ -14214,7 +14228,9 @@
       <c r="X70" s="19">
         <v>2</v>
       </c>
-      <c r="Y70" s="19"/>
+      <c r="Y70" s="19">
+        <v>3</v>
+      </c>
       <c r="AA70" s="22"/>
     </row>
     <row r="71" spans="2:27" x14ac:dyDescent="0.25">
@@ -14268,12 +14284,14 @@
         <v>8</v>
       </c>
       <c r="X71" s="19">
-        <v>5</v>
-      </c>
-      <c r="Y71" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="Y71" s="19">
+        <v>8</v>
+      </c>
       <c r="AA71" s="22">
         <f t="shared" ref="AA71:AA73" si="260">SUM(E71:Y71)</f>
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="72" spans="2:27" x14ac:dyDescent="0.25">
@@ -14416,15 +14434,15 @@
       </c>
       <c r="X73" s="20">
         <f t="shared" ref="X73" si="279">SUM(X67:X72)</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Y73" s="20">
         <f t="shared" ref="Y73" si="280">SUM(Y67:Y72)</f>
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="AA73" s="20">
         <f t="shared" si="260"/>
-        <v>516</v>
+        <v>546</v>
       </c>
     </row>
     <row r="74" spans="2:27" x14ac:dyDescent="0.25">
@@ -14510,11 +14528,11 @@
       </c>
       <c r="X74" s="18">
         <f t="shared" ref="X74" si="298">W74+X73</f>
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="Y74" s="18">
         <f t="shared" ref="Y74" si="299">X74+Y73</f>
-        <v>516</v>
+        <v>546</v>
       </c>
       <c r="AA74" s="5"/>
     </row>
@@ -14603,15 +14621,15 @@
       </c>
       <c r="X75" s="10">
         <f t="shared" si="300"/>
-        <v>2.04</v>
+        <v>2.2440000000000002</v>
       </c>
       <c r="Y75" s="10">
         <f t="shared" si="300"/>
-        <v>0.34</v>
+        <v>2.1760000000000002</v>
       </c>
       <c r="AA75" s="10">
         <f>SUM(E75:Y75)</f>
-        <v>35.088000000000001</v>
+        <v>37.128</v>
       </c>
     </row>
     <row r="76" spans="2:27" x14ac:dyDescent="0.25">
@@ -14702,11 +14720,11 @@
       </c>
       <c r="X76" s="10">
         <f t="shared" ref="X76" si="318">W76+X75</f>
-        <v>34.747999999999998</v>
+        <v>34.951999999999998</v>
       </c>
       <c r="Y76" s="10">
         <f t="shared" ref="Y76" si="319">X76+Y75</f>
-        <v>35.088000000000001</v>
+        <v>37.128</v>
       </c>
     </row>
     <row r="79" spans="2:27" x14ac:dyDescent="0.25">
@@ -15153,7 +15171,9 @@
       <c r="V86" s="19"/>
       <c r="W86" s="19"/>
       <c r="X86" s="19"/>
-      <c r="Y86" s="19"/>
+      <c r="Y86" s="19">
+        <v>5</v>
+      </c>
       <c r="AA86" s="22"/>
     </row>
     <row r="87" spans="2:27" x14ac:dyDescent="0.25">
@@ -15206,7 +15226,9 @@
       <c r="X87" s="19">
         <v>5</v>
       </c>
-      <c r="Y87" s="19"/>
+      <c r="Y87" s="19">
+        <v>5</v>
+      </c>
       <c r="AA87" s="22"/>
     </row>
     <row r="88" spans="2:27" x14ac:dyDescent="0.25">
@@ -15252,8 +15274,12 @@
       <c r="W88" s="19">
         <v>2</v>
       </c>
-      <c r="X88" s="19"/>
-      <c r="Y88" s="19"/>
+      <c r="X88" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y88" s="19">
+        <v>1</v>
+      </c>
       <c r="AA88" s="22"/>
     </row>
     <row r="89" spans="2:27" x14ac:dyDescent="0.25">
@@ -15303,10 +15329,12 @@
       <c r="X89" s="19">
         <v>1</v>
       </c>
-      <c r="Y89" s="19"/>
+      <c r="Y89" s="19">
+        <v>1</v>
+      </c>
       <c r="AA89" s="22">
         <f t="shared" ref="AA89:AA91" si="358">SUM(E89:Y89)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="90" spans="2:27" x14ac:dyDescent="0.25">
@@ -15345,13 +15373,17 @@
       <c r="U90" s="19">
         <v>5</v>
       </c>
-      <c r="V90" s="19"/>
-      <c r="W90" s="19"/>
+      <c r="V90" s="19">
+        <v>1</v>
+      </c>
+      <c r="W90" s="19">
+        <v>1</v>
+      </c>
       <c r="X90" s="19"/>
       <c r="Y90" s="19"/>
       <c r="AA90" s="22">
         <f t="shared" si="358"/>
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="2:27" x14ac:dyDescent="0.25">
@@ -15429,23 +15461,23 @@
       </c>
       <c r="V91" s="20">
         <f t="shared" ref="V91" si="375">SUM(V85:V90)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W91" s="20">
         <f t="shared" ref="W91" si="376">SUM(W85:W90)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X91" s="20">
         <f t="shared" ref="X91" si="377">SUM(X85:X90)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Y91" s="20">
         <f t="shared" ref="Y91" si="378">SUM(Y85:Y90)</f>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AA91" s="20">
         <f t="shared" si="358"/>
-        <v>122</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="2:27" x14ac:dyDescent="0.25">
@@ -15523,19 +15555,19 @@
       </c>
       <c r="V92" s="18">
         <f t="shared" ref="V92" si="394">U92+V91</f>
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="W92" s="18">
         <f t="shared" ref="W92" si="395">V92+W91</f>
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="X92" s="18">
         <f t="shared" ref="X92" si="396">W92+X91</f>
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="Y92" s="18">
         <f t="shared" ref="Y92" si="397">X92+Y91</f>
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="AA92" s="5"/>
     </row>
@@ -15616,23 +15648,23 @@
       </c>
       <c r="V93" s="10">
         <f t="shared" si="398"/>
-        <v>1.02</v>
+        <v>1.0880000000000001</v>
       </c>
       <c r="W93" s="10">
         <f t="shared" si="398"/>
-        <v>0.748</v>
+        <v>0.81599999999999995</v>
       </c>
       <c r="X93" s="10">
         <f t="shared" si="398"/>
-        <v>0.61199999999999999</v>
+        <v>0.68</v>
       </c>
       <c r="Y93" s="10">
         <f t="shared" si="398"/>
-        <v>0.20399999999999999</v>
+        <v>1.02</v>
       </c>
       <c r="AA93" s="10">
         <f>SUM(E93:Y93)</f>
-        <v>8.2959999999999994</v>
+        <v>9.3159999999999989</v>
       </c>
     </row>
     <row r="94" spans="2:27" x14ac:dyDescent="0.25">
@@ -15715,19 +15747,19 @@
       </c>
       <c r="V94" s="10">
         <f t="shared" ref="V94" si="414">U94+V93</f>
-        <v>6.7319999999999993</v>
+        <v>6.8</v>
       </c>
       <c r="W94" s="10">
         <f t="shared" ref="W94" si="415">V94+W93</f>
-        <v>7.4799999999999995</v>
+        <v>7.6159999999999997</v>
       </c>
       <c r="X94" s="10">
         <f t="shared" ref="X94" si="416">W94+X93</f>
-        <v>8.0919999999999987</v>
+        <v>8.2959999999999994</v>
       </c>
       <c r="Y94" s="10">
         <f t="shared" ref="Y94" si="417">X94+Y93</f>
-        <v>8.2959999999999994</v>
+        <v>9.3159999999999989</v>
       </c>
     </row>
     <row r="97" spans="2:27" x14ac:dyDescent="0.25">
@@ -16647,6 +16679,24 @@
       <c r="Y112" s="10">
         <f t="shared" ref="Y112" si="515">X112+Y111</f>
         <v>1.6999999999999997</v>
+      </c>
+    </row>
+    <row r="115" spans="25:27" x14ac:dyDescent="0.25">
+      <c r="Y115" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA115" s="21">
+        <f>SUM(AA14,AA28,AA45,AA62,AA80,AA98)</f>
+        <v>998</v>
+      </c>
+    </row>
+    <row r="116" spans="25:27" x14ac:dyDescent="0.25">
+      <c r="Y116" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA116" s="21">
+        <f>SUM(AA22,AA56,AA39,AA73,AA91,AA109)</f>
+        <v>889.5</v>
       </c>
     </row>
   </sheetData>
@@ -16707,7 +16757,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>

</xml_diff>